<commit_message>
fixed log manager : no doubles
</commit_message>
<xml_diff>
--- a/outputs/resultats.xlsx
+++ b/outputs/resultats.xlsx
@@ -538,7 +538,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1054,6 +1054,1022 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Adisa 2024</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-07-16 18:16:53</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Nigeria</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hôpital</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Monocentrique</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Étude avant-après</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Prospective</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Évaluer l'impact de l'intervention dirigée par un pharmacien sur l'adhérence médicamenteuse et l'utilisation des inhalateurs chez les patients asthmatiques et atteints de BPCO.</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>La différence dans le statut de contrôle de l'asthme ou l'état de santé clinique de la BPCO parmi les patients dans les deux groupes à la ligne de base et après la ligne de base.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Deux groupes</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Quasi-aléatoire</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Patients ambulatoires adultes âgés de 18 ans et plus avec un diagnostic principal d'asthme et/ou de BPCO, consentant volontairement à participer pleinement à l'étude jusqu'à son achèvement, et ayant un accès téléphonique actif.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Patients asthmatiques et/ou atteints de BPCO réservés pour une admission en hospitalisation, ceux qui ne prennent pas de médicaments liés à l'asthme/BPCO à un moment donné pendant la période de l'étude, et les patients non consentants.</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Insu simple (simple aveugle)</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Le paramètre principal est le changement dans le score CMAAS-12 et l'utilisation appropriée de l'appareil inhalateur, de la ligne de base à deux mois après la ligne de base parmi les patients des groupes de contrôle et d'intervention.</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Les résultats montrent une augmentation significative de l'adhérence médicamenteuse optimale de 33.3% à 63.3% dans le groupe d'intervention (p &lt; 0.001) et une amélioration significative de l'utilisation correcte du pMDI de 22.8% à 80.7% (p &lt; 0.001). Ces résultats sont statistiquement significatifs.</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Les outcomes secondaires incluent : 1) Le statut de contrôle de l'asthme, avec une augmentation significative des patients ayant un 'asthme bien contrôlé' dans le groupe d'intervention de 35.3% à 62.7% (p = 0.001). 2) Le statut de santé clinique spécifique à la BPCO, avec une augmentation significative des patients ayant un 'faible impact de la BPCO' dans le groupe d'intervention de 0% à 50% (p = 0.001). Ces résultats sont statistiquement significatifs.</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique consiste en des interventions éducatives et/ou cognitivo-comportementales dirigées par un pharmacien pour améliorer l'adhérence aux médicaments et l'utilisation correcte des inhalateurs chez les patients asthmatiques et atteints de BPCO.</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique se déroule à la clinique de pneumologie de l'hôpital universitaire de l'University College Hospital, Ibadan, Nigeria.</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Les acteurs de l'intervention sont les pharmaciens, les patients asthmatiques et atteints de BPCO, et les co-investigateurs de l'étude.</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>La durée de l'intervention est de 2 mois.</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Les limites de l'étude identifiées par les auteurs incluent la nature auto-déclarée de l'instrument CMAAS-12 avec ses limitations inhérentes telles que le biais de rappel ou de mémoire, l'utilisation d'un design quasi-expérimental avec une possibilité de biais de sélection/allocation, la durée perçue comme courte du suivi, et la taille totale de l'échantillon relativement petite, en particulier pour les patients atteints de BPCO.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Benny 2024</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-07-16 18:17:54</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Clinique externe</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Multicentrique</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>De août 2019 à septembre 2020, durée de 13 mois</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Étude observationnelle (sans intervention)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Rétrospective</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Analyser l'impact des rencontres téléphoniques de transition de soins par un pharmacien sur les taux de réadmission dans un ACO basé sur les soins primaires.</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>30-day readmission rate for targeted disease states, time to readmission, and readmission reason the same as previous discharge reason.</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Deux groupes</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Non aléatoire</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Patients de 65 ans ou plus, admis à l'hôpital ou au service des urgences d'août 2019 à septembre 2020, et ayant eu une tentative de rencontre téléphonique de transition de soins.</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Patients non suivis par les PCPs des trois bureaux de soins primaires de l'ACO, décédés à la sortie, ou transférés dans un établissement de soins spécialisés.</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Aucun insu</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Le paramètre principal est le taux de réadmission toutes causes confondues à 30 jours.</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Les résultats du paramètre principal montrent que les taux de réadmission à 30 jours étaient similaires entre ceux qui ont reçu une rencontre téléphonique de transition de soins et ceux qui ne l'ont pas reçue : 15.7% contre 28.2%. Ces résultats ne sont pas statistiquement significatifs (P = 0.059).</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Les outcomes secondaires incluent : 1) Le temps jusqu'à la réadmission, qui était plus élevé dans le groupe d'intervention du pharmacien mais non significatif (16 jours contre 6 jours; P = 0.058). 2) La raison de la réadmission étant la même que la raison de la sortie précédente, qui n'est pas significative (0% contre 20%).</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Le pharmacien effectue une réconciliation médicamenteuse, fournit des conseils appropriés, documente et envoie des recommandations au fournisseur via le dossier médical électronique.</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique se déroule dans un cadre de soins primaires basé sur une organisation de soins responsables (ACO) en Floride du Sud.</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>Les acteurs de l'intervention sont le pharmacien clinique, deux résidents en soins ambulatoires PGY2, et les patients ayant eu un contact téléphonique de transition de soins.</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Les appels téléphoniques durent entre 30 minutes et 1 heure selon la complexité du cas du patient.</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Les limites de l'étude identifiées par les auteurs incluent la taille d'échantillon limitée, la zone géographique limitée, la durée de l'étude, et la généralisation limitée aux personnes assurées avec accès aux spécialistes et installations. L'impact pourrait être plus grand chez ceux avec un accès limité aux soins de santé.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Abou 2025</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-07-16 18:19:48</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Les Pays-Bas</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pharmacie communautaire</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Multicentrique</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Début : novembre 2020, Fin : décembre 2021, Durée : 13 mois</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Essai contrôlé randomisé</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Prospective</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Le principal objectif de l'étude est d'évaluer si une formation axée sur la réalisation d'une revue de médication clinique orientée vers la déprescription entraîne une réduction de l'utilisation inappropriée de médicaments cardiovasculaires et antidiabétiques.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Les objectifs secondaires incluent le type de médication et le nombre d'interventions de déprescription proposées lors des réunions de suivi avec les médecins généralistes et les patients 1 à 4 semaines après la revue de médication clinique (T1).</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Deux groupes sont à l'étude.</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Aléatoire</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Les critères d'inclusion des participants sont : 70 ans ou plus, utilisation chronique de cinq médicaments ou plus, y compris au moins un médicament antihypertenseur ou antidiabétique, pression artérielle systolique mesurée récemment (&lt; 6 mois avant l'inclusion) &lt; 140 mmHg et/ou un niveau d'HbA1c &lt; 54 mmol/mol, et une espérance de vie de plus de 3 mois estimée par le médecin généraliste.</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Aucun insu</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Le paramètre principal est la proportion de patients avec un ou plusieurs médicaments cardiovasculaires et antidiabétiques déprescrits dans les 3 mois suivant la revue de médication clinique (CMR).</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>À T2, 32% des patients du groupe d'intervention et 26% du groupe de contrôle avaient un ou plusieurs médicaments cardiovasculaires ou antidiabétiques arrêtés. Ces résultats ne sont pas statistiquement significatifs (OR 1.4, CI 0.65–2.82, p = 0.413).</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Le outcome secondaire est le type de médicament et le nombre d'interventions de déprescription proposées lors des réunions de suivi avec les médecins généralistes et les patients 1 à 4 semaines après la CMR (T1). Les résultats montrent que des propositions de déprescription de médicaments cardiovasculaires et antidiabétiques ont été faites pour 55% des patients du groupe d'intervention et 46% du groupe de contrôle, ce qui n'est pas statistiquement significatif (p = 0.411). Concernant tous les médicaments, ces pourcentages étaient de 75% et 70%, respectivement, ce qui n'est pas statistiquement significatif (p = 0.752).</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique consiste en une formation des pharmaciens communautaires pour mener une revue de médication clinique axée sur la déprescription des médicaments cardiovasculaires et antidiabétiques.</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique se déroule dans les pharmacies communautaires aux Pays-Bas.</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>Les acteurs de l'intervention sont les pharmaciens communautaires, les médecins généralistes, les patients âgés de 70 ans ou plus, et potentiellement d'autres professionnels de santé comme les gériatres.</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>La durée de l'intervention est de 3 mois après la revue de médication clinique.</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Les limites de l'étude identifiées par les auteurs incluent la période d'inclusion qui a coïncidé avec la pandémie de COVID-19, rendant le processus d'inclusion difficile. Le nombre cible initial de patients par pharmacien n'a pas été atteint en raison des circonstances. Les résultats non significatifs peuvent être dus à une puissance insuffisante de l'étude. Un biais de sélection pourrait avoir eu lieu car les pharmaciens d'intervention pouvaient sélectionner des patients plus éligibles pour la déprescription. La collaboration avec les médecins généralistes était difficile en raison d'une pénurie de médecins et d'un manque de temps. La plupart des pharmaciens n'avaient pas accès directement aux données de pression artérielle ou d'HbA1c. Les effets de la déprescription ont été évalués seulement après 3 mois, sans données longitudinales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Adisa 2024</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-07-16 18:40:01</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Nigeria</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Hôpital</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Monocentrique</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Étude avant-après</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Prospective</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Évaluer l'impact de l'intervention dirigée par un pharmacien sur l'adhésion aux médicaments et l'utilisation des inhalateurs chez les patients asthmatiques et atteints de BPCO</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>La différence dans le statut de contrôle de l'asthme ou de la santé clinique de la BPCO parmi les patients dans les deux groupes à la ligne de base et après la ligne de base</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Deux groupes</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Quasi-aléatoire</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Patients ambulatoires adultes âgés de 18 ans et plus avec un diagnostic principal d'asthme et/ou de BPCO, consentant volontairement à participer pleinement à l'étude jusqu'à son achèvement, et ayant un accès téléphonique actif</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Patients asthmatiques et/ou atteints de BPCO réservés pour une admission en hospitalisation, ceux qui ne prennent pas de médicaments liés à l'asthme/BPCO à un moment quelconque pendant la période de l'étude, ainsi que les patients non consentants</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Insu simple (simple aveugle)</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Le paramètre principal est le changement dans le score CMAAS-12 et l'utilisation appropriée de l'appareil inhalateur, de la ligne de base à deux mois après la ligne de base parmi les patients des groupes de contrôle et d'intervention.</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Les résultats montrent une augmentation significative de l'adhérence médicamenteuse optimale dans le groupe d'intervention, passant de 20 (33.3%) à 38 (63.3%), p &lt; 0.001. De plus, l'utilisation correcte du pMDI est passée de 13 (22.8%) à 46 (80.7%) dans le groupe d'intervention, p &lt; 0.001. Ces résultats sont statistiquement significatifs.</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Les outcomes secondaires incluent : 1) Le statut de contrôle de l'asthme, mesuré par le test de contrôle de l'asthme (ACT). Dans le groupe d'intervention, la proportion de patients avec un asthme bien contrôlé est passée de 18 (35.3%) à 32 (62.7%), p = 0.001, ce qui est statistiquement significatif. 2) Le statut de santé clinique spécifique à la BPCO, mesuré par le test d'évaluation de la BPCO (CAT). Dans le groupe d'intervention, la proportion de patients avec un faible impact de la BPCO est passée de 0 (0.0%) à 7 (50.0%), p = 0.001, ce qui est statistiquement significatif.</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique consiste en des interventions éducatives et/ou cognitivo-comportementales dirigées par un pharmacien pour améliorer l'adhésion aux médicaments et l'utilisation correcte des inhalateurs chez les patients asthmatiques et atteints de BPCO.</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique se déroule à la clinique de pneumologie de l'hôpital universitaire de l'University College Hospital, Ibadan, Nigeria.</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Les acteurs de l'intervention sont les pharmaciens, les patients asthmatiques et atteints de BPCO, et les médecins traitants.</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>La durée de l'intervention est de 2 mois.</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>Les limites de l'étude identifiées par les auteurs incluent la nature auto-déclarée de l'instrument CMAAS-12 avec ses limitations inhérentes telles que le biais de rappel ou de mémoire, l'utilisation d'un design quasi-expérimental avec une possible sélection/allocation biaisée, la durée perçue comme courte du suivi, et la taille totale de l'échantillon relativement petite, en particulier pour les patients atteints de BPCO.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Benny 2024</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-07-16 18:41:03</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Autre</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Multicentrique</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Début : Août 2019, Fin : Septembre 2020, Durée : Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Étude observationnelle (sans intervention)</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Rétrospective</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Analyser l'impact des rencontres téléphoniques de transitions de soins (TOC) par un pharmacien sur les taux de réadmission dans un ACO basé sur les soins primaires.</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>30-day readmission rate for targeted disease states, time to readmission, and readmission reason the same as previous discharge reason.</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Deux groupes</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Non aléatoire</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Patients de 65 ans ou plus, admis à l'hôpital ou au service des urgences d'août 2019 à septembre 2020, et ayant eu une tentative de rencontre téléphonique TOC.</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Patients n'étant plus sous la responsabilité des PCPs dans les trois bureaux de soins primaires de l'ACO, décédés à la sortie, ou transférés dans un établissement de soins spécialisés.</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Aucun insu</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Le paramètre principal est le taux de réadmission toutes causes confondues à 30 jours.</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Les résultats du paramètre principal montrent que les taux de réadmission à 30 jours étaient similaires entre ceux qui ont reçu une rencontre téléphonique de transition de soins et ceux qui ne l'ont pas reçue : 15.7% contre 28.2%. Ces résultats ne sont pas statistiquement significatifs (P = 0.059).</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Les outcomes secondaires incluent : 1) Le temps jusqu'à la réadmission, qui était plus élevé dans le groupe d'intervention du pharmacien mais non significatif (16 jours contre 6 jours; P = 0.058). 2) La raison de la réadmission étant la même que la raison de la sortie précédente, avec 0% dans le groupe contacté et 20% dans le groupe non contacté, mais la significativité statistique n'est pas précisée.</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Le pharmacien effectue des appels téléphoniques de transition de soins (TOC), réalise une réconciliation médicamenteuse, fournit des conseils appropriés, et envoie des recommandations au fournisseur via le dossier médical électronique (EMR).</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique se déroule dans trois bureaux de soins primaires d'une organisation de soins responsables (ACO) en Floride du Sud.</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Les acteurs de l'intervention sont le pharmacien clinique, deux résidents en soins ambulatoires PGY2, les patients, et les fournisseurs de soins primaires (médecins, assistants médicaux, et une infirmière praticienne avancée).</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Les appels téléphoniques durent entre 30 minutes et 1 heure selon la complexité du cas du patient.</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>Les limites de l'étude identifiées par les auteurs incluent la taille d'échantillon limitée, la zone géographique limitée, la durée de l'étude, et la généralisation limitée aux personnes assurées avec accès à des spécialistes et des installations. L'impact d'une rencontre téléphonique de transition de soins par un pharmacien pourrait être plus important chez ceux ayant un accès limité aux soins de santé.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Abou 2025</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-07-16 18:42:58</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Pays-Bas</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Pharmacie communautaire</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Multicentrique</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Début : novembre 2020, Fin : décembre 2021, Durée : environ 1 an</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Essai contrôlé randomisé</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Prospective</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Le principal objectif de l'étude est d'évaluer si une formation axée sur la réalisation d'une revue de médication clinique orientée vers la déprescription entraîne une réduction de l'utilisation inappropriée de médicaments cardiovasculaires et antidiabétiques.</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Les objectifs secondaires incluent le type de médication et le nombre d'interventions de déprescription proposées lors des réunions de suivi avec les médecins généralistes et les patients 1 à 4 semaines après la revue de médication clinique (T1).</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Deux groupes sont à l'étude.</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Aléatoire</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Les critères d'inclusion des participants sont : 70 ans ou plus, utilisation chronique de cinq médicaments ou plus, y compris au moins un médicament antihypertenseur ou antidiabétique, pression artérielle systolique mesurée récemment (&lt; 6 mois avant l'inclusion) &lt; 140 mmHg et/ou un niveau d'HbA1c &lt; 54 mmol/mol, et une espérance de vie de plus de 3 mois estimée par le médecin généraliste.</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Aucun insu</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Le paramètre principal est la proportion de patients avec un ou plusieurs médicaments cardiovasculaires et antidiabétiques déprescrits dans les 3 mois suivant la revue de médication clinique (CMR).</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>À T2, 32% des patients du groupe d'intervention et 26% du groupe de contrôle avaient un ou plusieurs médicaments cardiovasculaires ou antidiabétiques arrêtés. Ces résultats ne sont pas statistiquement significatifs (OR 1.4, CI 0.65–2.82, p = 0.413).</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Le ou les outcome(s) secondaire(s) incluent : 1. Le type de médicament et le nombre d'interventions de déprescription proposées lors des réunions de suivi avec les médecins généralistes et les patients 1 à 4 semaines après le CMR (T1). Résultats : 55% des patients du groupe d'intervention et 46% du groupe de contrôle ont eu des propositions de déprescription de médicaments cardiovasculaires et antidiabétiques. Ces résultats ne sont pas statistiquement significatifs (p = 0.411). 2. Concernant tous les médicaments, 75% des patients du groupe d'intervention et 70% du groupe de contrôle ont eu des propositions de déprescription. Ces résultats ne sont pas statistiquement significatifs (p = 0.752).</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique consiste en une formation des pharmaciens communautaires pour mener une revue de médication clinique axée sur la déprescription des médicaments cardiovasculaires et antidiabétiques.</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique se déroule dans les pharmacies communautaires aux Pays-Bas.</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>Les acteurs de l'intervention sont les pharmaciens communautaires, les médecins généralistes, les patients âgés de 70 ans ou plus, et potentiellement d'autres professionnels de santé comme les gériatres.</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>La durée de l'intervention est de 3 mois après la revue de médication clinique.</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>Les limites de l'étude identifiées par les auteurs incluent la période d'inclusion qui a coïncidé avec la pandémie de COVID-19, rendant le processus d'inclusion difficile. Le nombre cible initial de patients par CP n'a pas été atteint en raison des circonstances. La non-significativité des résultats pourrait être due à une puissance insuffisante de l'étude. Un biais de sélection pourrait avoir eu lieu car les CP de l'intervention pouvaient sélectionner des patients plus éligibles pour la déprescription. La collaboration avec les médecins généralistes était de plus en plus difficile en raison d'une pénurie de médecins et d'un manque de temps. La plupart des CP n'avaient pas d'accès direct aux données de pression artérielle ou d'HbA1c. Les effets de la déprescription ont été évalués seulement après 3 mois, sans données longitudinales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Adisa 2024</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-07-16 18:47:54</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Nigeria</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Hôpital</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Monocentrique</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Étude avant-après</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Prospective</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Évaluer l'impact de l'intervention dirigée par un pharmacien sur l'adhésion aux médicaments et l'utilisation des inhalateurs chez les patients asthmatiques et atteints de BPCO</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>La différence dans le statut de contrôle de l'asthme ou de la santé clinique de la BPCO parmi les patients dans les deux groupes au début et après l'intervention</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Deux groupes</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Quasi-aléatoire</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Patients ambulatoires adultes âgés de 18 ans et plus avec un diagnostic principal d'asthme et/ou de BPCO, consentant à participer pleinement à l'étude, et ayant un accès téléphonique actif</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Patients asthmatiques et/ou atteints de BPCO réservés pour une admission en hospitalisation, ceux qui ne prennent pas de médicaments liés à l'asthme/BPCO à un moment donné pendant l'étude, et les patients non consentants</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Insu simple (simple aveugle)</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Le paramètre principal est le changement dans le score CMAAS-12 et l'utilisation appropriée de l'appareil inhalateur, de la ligne de base à deux mois après la ligne de base parmi les patients des groupes de contrôle et d'intervention.</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Les résultats montrent une augmentation significative de l'adhérence médicamenteuse optimale dans le groupe d'intervention, passant de 33.3% à 63.3% (p &lt; 0.001). De plus, l'utilisation correcte du pMDI est passée de 22.8% à 80.7% dans le groupe d'intervention (p &lt; 0.001). Ces résultats sont statistiquement significatifs.</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Les outcomes secondaires incluent : 1) Le statut de contrôle de l'asthme, mesuré par le test de contrôle de l'asthme (ACT). Dans le groupe d'intervention, la proportion de patients avec un asthme bien contrôlé est passée de 35.3% à 62.7% (p = 0.001), ce qui est statistiquement significatif. 2) Le statut de santé clinique spécifique à la BPCO, mesuré par le test d'évaluation de la BPCO (CAT). Dans le groupe d'intervention, la proportion de patients avec un faible impact de la BPCO est passée de 0% à 50% (p = 0.001), ce qui est statistiquement significatif.</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique consiste en des interventions éducatives et/ou cognitivo-comportementales dirigées par un pharmacien pour améliorer l'adhésion aux médicaments et l'utilisation correcte des inhalateurs chez les patients asthmatiques et atteints de BPCO.</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique se déroule à la clinique de pneumologie de l'hôpital universitaire de l'University College Hospital, Ibadan, Nigeria.</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>Les acteurs de l'intervention sont les pharmaciens, les patients asthmatiques et atteints de BPCO, et les co-investigateurs de l'étude.</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>La durée de l'intervention est de 2 mois.</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>Les limites de l'étude identifiées par les auteurs incluent la nature auto-déclarée de l'instrument CMAAS-12 avec ses limitations inhérentes telles que le biais de rappel ou de mémoire, l'utilisation d'un design quasi-expérimental avec une possible sélection/allocation biaisée, la durée perçue comme courte du suivi, et la taille totale de l'échantillon relativement petite, en particulier pour les patients atteints de BPCO.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Benny 2024</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-07-16 18:48:55</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Clinique externe</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Multicentrique</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Début : Août 2019, Fin : Septembre 2020, Durée : Non précisé dans l'article</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Étude observationnelle (sans intervention)</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Rétrospective</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Analyser l'impact des rencontres téléphoniques de transition de soins par un pharmacien sur les taux de réadmission dans un ACO basé sur les soins primaires.</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>30-day readmission rate for targeted disease states, time to readmission, and readmission reason the same as previous discharge reason.</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Deux groupes</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Non aléatoire</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Patients de 65 ans ou plus, admis à l'hôpital ou au service d'urgence d'août 2019 à septembre 2020, et ayant eu une tentative de rencontre téléphonique de transition de soins.</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Patients non suivis par les PCPs des trois bureaux de soins primaires de l'ACO, décédés à la sortie, ou transférés dans un établissement de soins spécialisés.</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Aucun insu</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Le paramètre principal est le taux de réadmission toutes causes confondues à 30 jours.</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Les résultats du paramètre principal montrent que les taux de réadmission à 30 jours étaient similaires entre ceux qui ont reçu une rencontre téléphonique de transition de soins (15.7%) et ceux qui ne l'ont pas reçue (28.2%). Ces résultats ne sont pas statistiquement significatifs (P = 0.059).</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Les outcomes secondaires incluent : 1) Le temps jusqu'à la réadmission, qui était plus élevé dans le groupe d'intervention du pharmacien (16 jours) par rapport au groupe sans intervention (6 jours), mais ce n'était pas significatif (P = 0.058). 2) La raison de la réadmission étant la même que la raison de la sortie précédente, avec 0% dans le groupe contacté et 20% dans le groupe non contacté, mais la significativité statistique n'est pas précisée.</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Le pharmacien effectue une réconciliation médicamenteuse, fournit des conseils appropriés, documente et envoie des recommandations au fournisseur via le dossier médical électronique.</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>L'intervention pharmaceutique se déroule dans un cadre de soins primaires basé sur une organisation de soins responsables (ACO) en Floride du Sud.</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>Les acteurs de l'intervention sont le pharmacien clinique, deux résidents en soins ambulatoires PGY2, et les patients ayant eu un contact téléphonique de transition de soins.</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>Les appels téléphoniques durent entre 30 minutes et 1 heure selon la complexité du cas du patient.</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>Les limites de l'étude identifiées par les auteurs incluent la taille d'échantillon limitée, la zone géographique limitée, la durée de l'étude, et la généralisation limitée aux personnes assurées avec accès à des spécialistes et des installations. L'impact d'une rencontre téléphonique de transition de soins par un pharmacien pourrait être plus grand chez ceux ayant un accès limité aux soins de santé.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>

</xml_diff>